<commit_message>
Unit 3 bonus work
Unit 3 bonus work
</commit_message>
<xml_diff>
--- a/Unit_03/Assignment/Assignment_03.xlsx
+++ b/Unit_03/Assignment/Assignment_03.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E42A77-6716-4A80-95A2-0E0DFB2EC6DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1310EC-CD99-4FE2-8335-FE4AD6DD8088}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="2130" windowWidth="29100" windowHeight="17310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8295" yWindow="2595" windowWidth="28350" windowHeight="19335" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tank" sheetId="3" r:id="rId1"/>
     <sheet name="Fertilizer" sheetId="1" r:id="rId2"/>
     <sheet name="Fencing" sheetId="2" r:id="rId3"/>
+    <sheet name="Toys" sheetId="4" r:id="rId4"/>
+    <sheet name="Mines" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="2" hidden="1">Fencing!$D$6:$D$8</definedName>
@@ -135,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>x1</t>
   </si>
@@ -195,6 +197,30 @@
   </si>
   <si>
     <t>Coef:</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>Truck</t>
+  </si>
+  <si>
+    <t>Turtle</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>Rubber</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -206,7 +232,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +312,27 @@
       <i/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -381,7 +428,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -414,6 +461,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -847,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8A2B7F-7875-42BA-8179-C3B137595E0E}">
-  <dimension ref="B4:J14"/>
+  <dimension ref="B4:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,6 +1004,12 @@
         <v>111.34480842618285</v>
       </c>
     </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="20"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -963,7 +1022,7 @@
   <dimension ref="B3:J10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFAD3EB8-965E-4758-9AD9-2BB35957C59A}">
   <dimension ref="A3:J9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,6 +1166,9 @@
       <c r="G4" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="H4" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1211,4 +1273,182 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E99644-94F8-4BA7-B816-67A2A47EEB3F}">
+  <dimension ref="B4:L9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="J5">
+        <f>H5*G5+F5*E5+D5*C5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="22">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="J6">
+        <f>H6*G6+F6*E6+D6*C6</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="22">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7">
+        <v>0.6</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="J7">
+        <f t="shared" ref="J7" si="0">H7*G7+F7*E7+D7*C7</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="22">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="J8">
+        <f>H8*G8+F8*E8+D8*C8</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="J9">
+        <f>H9*G9+F9*E9+D9*C9</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="22">
+        <v>164000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0946960-F8C5-491A-9C81-73992497BA7F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>